<commit_message>
Code changes till 08-07-2025 03:15pm
</commit_message>
<xml_diff>
--- a/Documents/Thannickal_Bakers_Working.xlsx
+++ b/Documents/Thannickal_Bakers_Working.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Globocon\BMS\Application\BakeryManagementSystem\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D2BBE8-971C-4D15-9DFF-4846DAD076D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8B0451-86A6-4BA9-9AF8-906C0F01DDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" firstSheet="1" activeTab="4" xr2:uid="{9EA4B1FA-7DD5-4CCE-97E0-9A7AE5A0A6E4}"/>
   </bookViews>
@@ -53,7 +53,6 @@
     <externalReference r:id="rId36"/>
   </externalReferences>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1032,9 +1031,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1593,7 +1593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1872,12 +1872,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1897,9 +1891,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1940,6 +1931,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2526,11 +2521,11 @@
         <v>235</v>
       </c>
       <c r="B5" s="92"/>
-      <c r="C5" s="134" t="s">
+      <c r="C5" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="D5" s="134"/>
-      <c r="E5" s="135"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="132"/>
       <c r="G5">
         <v>1</v>
       </c>
@@ -3110,10 +3105,10 @@
       <c r="Q2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="137" t="s">
+      <c r="S2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="T2" s="137"/>
+      <c r="T2" s="134"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -3182,8 +3177,8 @@
         <f>0.04*B3</f>
         <v>0</v>
       </c>
-      <c r="S3" s="137"/>
-      <c r="T3" s="137"/>
+      <c r="S3" s="134"/>
+      <c r="T3" s="134"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -3600,10 +3595,10 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G1" s="22"/>
-      <c r="O1" s="142" t="s">
+      <c r="O1" s="139" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="142"/>
+      <c r="P1" s="139"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3654,10 +3649,10 @@
       <c r="P2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="R2" s="137" t="s">
+      <c r="R2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="S2" s="137"/>
+      <c r="S2" s="134"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -3722,8 +3717,8 @@
         <f>$B3*0.005</f>
         <v>0</v>
       </c>
-      <c r="R3" s="137"/>
-      <c r="S3" s="137"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="134"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -3837,8 +3832,8 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G1" s="22"/>
-      <c r="M1" s="143"/>
-      <c r="N1" s="143"/>
+      <c r="M1" s="140"/>
+      <c r="N1" s="140"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3886,10 +3881,10 @@
       <c r="O2" s="106" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="137" t="s">
+      <c r="P2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="Q2" s="137"/>
+      <c r="Q2" s="134"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -3950,8 +3945,8 @@
         <f>B3*0.13</f>
         <v>0.32500000000000001</v>
       </c>
-      <c r="P3" s="137"/>
-      <c r="Q3" s="137"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -4069,10 +4064,10 @@
       <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="137" t="s">
+      <c r="F2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="G2" s="137"/>
+      <c r="G2" s="134"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
@@ -4089,8 +4084,8 @@
         <f>$B3*0.01</f>
         <v>0.06</v>
       </c>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -4151,11 +4146,11 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F1" s="22"/>
-      <c r="K1" s="144" t="s">
+      <c r="K1" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -4197,10 +4192,10 @@
       <c r="M2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="137" t="s">
+      <c r="O2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="P2" s="137"/>
+      <c r="P2" s="134"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
@@ -4253,8 +4248,8 @@
         <f>$B3*0.005</f>
         <v>0</v>
       </c>
-      <c r="O3" s="137"/>
-      <c r="P3" s="137"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -4362,10 +4357,10 @@
       <c r="F2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="137" t="s">
+      <c r="H2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="I2" s="137"/>
+      <c r="I2" s="134"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
@@ -4390,8 +4385,8 @@
         <f>$B3*0.24</f>
         <v>0.96</v>
       </c>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -4471,10 +4466,10 @@
       <c r="F2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="137" t="s">
+      <c r="H2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="I2" s="137"/>
+      <c r="I2" s="134"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
@@ -4499,8 +4494,8 @@
         <f>$B3*0.24</f>
         <v>0</v>
       </c>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -4580,10 +4575,10 @@
       <c r="F2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="137">
+      <c r="H2" s="134">
         <v>1</v>
       </c>
-      <c r="I2" s="137"/>
+      <c r="I2" s="134"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
@@ -4608,8 +4603,8 @@
         <f>$B3*0.175</f>
         <v>0.17499999999999999</v>
       </c>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -4695,10 +4690,10 @@
       <c r="G2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="137" t="s">
+      <c r="I2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="J2" s="137"/>
+      <c r="J2" s="134"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
@@ -4727,8 +4722,8 @@
         <f>$B3*0.0555</f>
         <v>0</v>
       </c>
-      <c r="I3" s="137"/>
-      <c r="J3" s="137"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -4843,10 +4838,10 @@
       <c r="M2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="137" t="s">
+      <c r="O2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="P2" s="137"/>
+      <c r="P2" s="134"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -4896,8 +4891,8 @@
         <f t="shared" ref="M3:M14" si="3">D3*1</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="O3" s="137"/>
-      <c r="P3" s="137"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
       <c r="S3" s="51"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -5699,23 +5694,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="133" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
       <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U2" s="137" t="s">
+      <c r="U2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="V2" s="137"/>
+      <c r="V2" s="134"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
@@ -5766,8 +5761,8 @@
       <c r="S3" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="U3" s="137"/>
-      <c r="V3" s="137"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="57">
@@ -6833,12 +6828,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N1" s="141" t="s">
+      <c r="N1" s="138" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="141"/>
-      <c r="P1" s="141"/>
-      <c r="Q1" s="141"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6892,10 +6887,10 @@
       <c r="Q2" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="137" t="s">
+      <c r="S2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="T2" s="137"/>
+      <c r="T2" s="134"/>
       <c r="U2" s="51"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -6965,8 +6960,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S3" s="137"/>
-      <c r="T3" s="137"/>
+      <c r="S3" s="134"/>
+      <c r="T3" s="134"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -7135,10 +7130,10 @@
       <c r="O2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="137" t="s">
+      <c r="Q2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="R2" s="137"/>
+      <c r="R2" s="134"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -7199,8 +7194,8 @@
         <f>$B3*0.0053</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="137"/>
-      <c r="R3" s="137"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -7327,10 +7322,10 @@
       <c r="F2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="137" t="s">
+      <c r="H2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="I2" s="137"/>
+      <c r="I2" s="134"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -7355,8 +7350,8 @@
         <f>$B3*0.0022</f>
         <v>0</v>
       </c>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -7428,11 +7423,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K1" s="144" t="s">
+      <c r="K1" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -7474,10 +7469,10 @@
       <c r="M2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="Q2" s="137" t="s">
+      <c r="Q2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="R2" s="137"/>
+      <c r="R2" s="134"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -7530,8 +7525,8 @@
         <f>$B3*0.0025</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="137"/>
-      <c r="R3" s="137"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -7638,11 +7633,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K1" s="144" t="s">
+      <c r="K1" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -7684,10 +7679,10 @@
       <c r="M2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="137" t="s">
+      <c r="P2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="Q2" s="137"/>
+      <c r="Q2" s="134"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -7740,8 +7735,8 @@
         <f>$B3*0.00375</f>
         <v>0</v>
       </c>
-      <c r="P3" s="137"/>
-      <c r="Q3" s="137"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -7849,11 +7844,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L1" s="144" t="s">
+      <c r="L1" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -7898,10 +7893,10 @@
       <c r="N2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="137" t="s">
+      <c r="P2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="Q2" s="137"/>
+      <c r="Q2" s="134"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -7958,8 +7953,8 @@
         <f>$B3*0.0025</f>
         <v>0</v>
       </c>
-      <c r="P3" s="137"/>
-      <c r="Q3" s="137"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -8072,11 +8067,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L1" s="144" t="s">
+      <c r="L1" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -8121,10 +8116,10 @@
       <c r="N2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="137" t="s">
+      <c r="P2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="Q2" s="137"/>
+      <c r="Q2" s="134"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -8181,8 +8176,8 @@
         <f>$B3*0.0025</f>
         <v>0</v>
       </c>
-      <c r="P3" s="137"/>
-      <c r="Q3" s="137"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -8295,11 +8290,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L1" s="144" t="s">
+      <c r="L1" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -8344,10 +8339,10 @@
       <c r="N2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="137" t="s">
+      <c r="P2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="Q2" s="137"/>
+      <c r="Q2" s="134"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -8404,8 +8399,8 @@
         <f>$B3*0.0025</f>
         <v>0</v>
       </c>
-      <c r="P3" s="137"/>
-      <c r="Q3" s="137"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -8528,10 +8523,10 @@
       <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="137" t="s">
+      <c r="H2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="I2" s="137"/>
+      <c r="I2" s="134"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -8556,8 +8551,8 @@
         <f>$B3*0.0076</f>
         <v>0</v>
       </c>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -8687,10 +8682,10 @@
       <c r="R2" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="T2" s="137" t="s">
+      <c r="T2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="U2" s="137"/>
+      <c r="U2" s="134"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -8763,8 +8758,8 @@
         <f>$B3*0.08</f>
         <v>0</v>
       </c>
-      <c r="T3" s="137"/>
-      <c r="U3" s="137"/>
+      <c r="T3" s="134"/>
+      <c r="U3" s="134"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -8901,33 +8896,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="135" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
-      <c r="O1" s="139"/>
-      <c r="P1" s="139"/>
-      <c r="Q1" s="139"/>
-      <c r="R1" s="139"/>
-      <c r="S1" s="140"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
+      <c r="Q1" s="136"/>
+      <c r="R1" s="136"/>
+      <c r="S1" s="137"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U2" s="137" t="s">
+      <c r="U2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="V2" s="137"/>
+      <c r="V2" s="134"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
@@ -8978,8 +8973,8 @@
       <c r="S3" s="56" t="s">
         <v>190</v>
       </c>
-      <c r="U3" s="137"/>
-      <c r="V3" s="137"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="57">
@@ -10171,10 +10166,10 @@
       <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="137" t="s">
+      <c r="H2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="I2" s="137"/>
+      <c r="I2" s="134"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -10196,8 +10191,8 @@
         <v>0.2</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -10341,10 +10336,10 @@
       <c r="D2" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="137" t="s">
+      <c r="F2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="G2" s="137"/>
+      <c r="G2" s="134"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -10361,8 +10356,8 @@
         <f>$B3*0.35</f>
         <v>0</v>
       </c>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -10456,8 +10451,8 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L1" s="22"/>
-      <c r="N1" s="141"/>
-      <c r="O1" s="141"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -10502,10 +10497,10 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="137" t="s">
+      <c r="Q2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="R2" s="137"/>
+      <c r="R2" s="134"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -10561,8 +10556,8 @@
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="137"/>
-      <c r="R3" s="137"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C4" s="10"/>
@@ -15992,14 +15987,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q2" s="137" t="s">
+      <c r="Q2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="R2" s="137"/>
+      <c r="R2" s="134"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q3" s="137"/>
-      <c r="R3" s="137"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
@@ -17379,8 +17374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D55B50-A414-40E8-B274-E34251BCB63C}">
   <dimension ref="A2:Y75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="133" zoomScaleNormal="231" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="133" zoomScaleNormal="231" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17467,10 +17462,10 @@
       <c r="T2" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="V2" s="137" t="s">
+      <c r="V2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="W2" s="137"/>
+      <c r="W2" s="134"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -17521,8 +17516,8 @@
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
       <c r="T3" s="15"/>
-      <c r="V3" s="137"/>
-      <c r="W3" s="137"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="134"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -19176,34 +19171,34 @@
       <c r="B41" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="120">
+      <c r="C41" s="143">
         <v>4.2857142857142858E-2</v>
       </c>
-      <c r="D41" s="120">
+      <c r="D41" s="143">
         <v>3.7500000000000006E-2</v>
       </c>
-      <c r="E41" s="121">
+      <c r="E41" s="143">
         <v>0.12</v>
       </c>
-      <c r="F41" s="122">
+      <c r="F41" s="143">
         <v>0.125</v>
       </c>
-      <c r="G41" s="122">
+      <c r="G41" s="143">
         <v>0.04</v>
       </c>
-      <c r="H41" s="117">
+      <c r="H41" s="142">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I41" s="123">
+      <c r="I41" s="142">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="J41" s="117">
+      <c r="J41" s="142">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="K41" s="117">
+      <c r="K41" s="142">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="L41" s="117">
+      <c r="L41" s="142">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="M41" s="117"/>
@@ -19217,30 +19212,45 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="117"/>
-      <c r="B42" s="124" t="s">
+      <c r="B42" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="122">
+      <c r="C42" s="143">
         <f>(C41*580)/1000</f>
         <v>2.4857142857142859E-2</v>
       </c>
-      <c r="D42" s="120">
+      <c r="D42" s="143">
         <v>2.1750000000000002E-2</v>
       </c>
-      <c r="E42" s="121">
+      <c r="E42" s="143">
         <v>6.9599999999999995E-2</v>
       </c>
-      <c r="F42" s="122">
+      <c r="F42" s="143">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="G42" s="122">
+      <c r="G42" s="143">
         <v>2.3199999999999998E-2</v>
       </c>
-      <c r="H42" s="117"/>
-      <c r="I42" s="117"/>
-      <c r="J42" s="117"/>
-      <c r="K42" s="117"/>
-      <c r="L42" s="117"/>
+      <c r="H42" s="142">
+        <f>(H41*580)/1000</f>
+        <v>1.9720000000000001E-2</v>
+      </c>
+      <c r="I42" s="142">
+        <f t="shared" ref="I42:L42" si="27">(I41*580)/1000</f>
+        <v>2.0300000000000002E-2</v>
+      </c>
+      <c r="J42" s="142">
+        <f t="shared" si="27"/>
+        <v>1.9720000000000001E-2</v>
+      </c>
+      <c r="K42" s="142">
+        <f t="shared" si="27"/>
+        <v>1.9720000000000001E-2</v>
+      </c>
+      <c r="L42" s="142">
+        <f t="shared" si="27"/>
+        <v>1.9720000000000001E-2</v>
+      </c>
       <c r="M42" s="117"/>
       <c r="N42" s="117"/>
       <c r="O42" s="117"/>
@@ -19255,27 +19265,42 @@
       <c r="B43" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="122">
+      <c r="C43" s="143">
         <f>(C41*20)/1000</f>
         <v>8.5714285714285721E-4</v>
       </c>
-      <c r="D43" s="120">
+      <c r="D43" s="143">
         <v>7.5000000000000012E-4</v>
       </c>
-      <c r="E43" s="121">
+      <c r="E43" s="143">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="F43" s="122">
+      <c r="F43" s="143">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="G43" s="122">
+      <c r="G43" s="143">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="H43" s="117"/>
-      <c r="I43" s="117"/>
-      <c r="J43" s="117"/>
-      <c r="K43" s="117"/>
-      <c r="L43" s="117"/>
+      <c r="H43" s="142">
+        <f>(H41*20)/1000</f>
+        <v>6.8000000000000005E-4</v>
+      </c>
+      <c r="I43" s="142">
+        <f>(I41*20)/1000</f>
+        <v>7.000000000000001E-4</v>
+      </c>
+      <c r="J43" s="142">
+        <f>(J41*20)/1000</f>
+        <v>6.8000000000000005E-4</v>
+      </c>
+      <c r="K43" s="142">
+        <f>(K41*20)/1000</f>
+        <v>6.8000000000000005E-4</v>
+      </c>
+      <c r="L43" s="142">
+        <f>(L41*20)/1000</f>
+        <v>6.8000000000000005E-4</v>
+      </c>
       <c r="M43" s="117"/>
       <c r="N43" s="117"/>
       <c r="O43" s="117"/>
@@ -19290,27 +19315,42 @@
       <c r="B44" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="122">
+      <c r="C44" s="143">
         <f>(C41*50)/1000</f>
         <v>2.142857142857143E-3</v>
       </c>
-      <c r="D44" s="120">
+      <c r="D44" s="143">
         <v>1.8750000000000001E-3</v>
       </c>
-      <c r="E44" s="121">
+      <c r="E44" s="143">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F44" s="122">
+      <c r="F44" s="143">
         <v>6.2500000000000003E-3</v>
       </c>
-      <c r="G44" s="122">
+      <c r="G44" s="143">
         <v>2E-3</v>
       </c>
-      <c r="H44" s="117"/>
-      <c r="I44" s="117"/>
-      <c r="J44" s="117"/>
-      <c r="K44" s="117"/>
-      <c r="L44" s="117"/>
+      <c r="H44" s="142">
+        <f>(H41*50)/1000</f>
+        <v>1.7000000000000001E-3</v>
+      </c>
+      <c r="I44" s="142">
+        <f t="shared" ref="I44:L44" si="28">(I41*50)/1000</f>
+        <v>1.7500000000000003E-3</v>
+      </c>
+      <c r="J44" s="142">
+        <f t="shared" si="28"/>
+        <v>1.7000000000000001E-3</v>
+      </c>
+      <c r="K44" s="142">
+        <f t="shared" si="28"/>
+        <v>1.7000000000000001E-3</v>
+      </c>
+      <c r="L44" s="142">
+        <f t="shared" si="28"/>
+        <v>1.7000000000000001E-3</v>
+      </c>
       <c r="M44" s="117"/>
       <c r="N44" s="117"/>
       <c r="O44" s="117"/>
@@ -19322,38 +19362,38 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="117"/>
-      <c r="B45" s="124" t="s">
+      <c r="B45" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="122">
+      <c r="C45" s="143">
         <f>C41*1</f>
         <v>4.2857142857142858E-2</v>
       </c>
-      <c r="D45" s="120">
+      <c r="D45" s="143">
         <v>3.7500000000000006E-2</v>
       </c>
-      <c r="E45" s="121">
+      <c r="E45" s="143">
         <v>0.12</v>
       </c>
-      <c r="F45" s="122">
+      <c r="F45" s="143">
         <v>0.125</v>
       </c>
-      <c r="G45" s="122">
+      <c r="G45" s="143">
         <v>0.04</v>
       </c>
-      <c r="H45" s="122">
+      <c r="H45" s="142">
         <v>0.53400000000000003</v>
       </c>
-      <c r="I45" s="122">
+      <c r="I45" s="142">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="J45" s="122">
+      <c r="J45" s="142">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="K45" s="122">
+      <c r="K45" s="142">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="L45" s="122">
+      <c r="L45" s="142">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="M45" s="117"/>
@@ -19367,32 +19407,47 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="117"/>
-      <c r="B46" s="124" t="s">
+      <c r="B46" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="122">
+      <c r="C46" s="143">
         <f>(C41*5)/1000</f>
         <v>2.142857142857143E-4</v>
       </c>
-      <c r="D46" s="120">
+      <c r="D46" s="143">
         <v>1.8750000000000003E-4</v>
       </c>
-      <c r="E46" s="121">
+      <c r="E46" s="143">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F46" s="122">
+      <c r="F46" s="143">
         <v>6.2500000000000001E-4</v>
       </c>
-      <c r="G46" s="122">
+      <c r="G46" s="143">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="H46" s="125"/>
-      <c r="I46" s="125"/>
-      <c r="J46" s="125"/>
-      <c r="K46" s="125"/>
-      <c r="L46" s="125"/>
-      <c r="M46" s="125"/>
-      <c r="N46" s="125"/>
+      <c r="H46" s="142">
+        <f>(H41*5)/1000</f>
+        <v>1.7000000000000001E-4</v>
+      </c>
+      <c r="I46" s="142">
+        <f t="shared" ref="I46:L46" si="29">(I41*5)/1000</f>
+        <v>1.7500000000000003E-4</v>
+      </c>
+      <c r="J46" s="142">
+        <f t="shared" si="29"/>
+        <v>1.7000000000000001E-4</v>
+      </c>
+      <c r="K46" s="142">
+        <f t="shared" si="29"/>
+        <v>1.7000000000000001E-4</v>
+      </c>
+      <c r="L46" s="142">
+        <f t="shared" si="29"/>
+        <v>1.7000000000000001E-4</v>
+      </c>
+      <c r="M46" s="123"/>
+      <c r="N46" s="123"/>
       <c r="O46" s="117"/>
       <c r="P46" s="117"/>
       <c r="Q46" s="117"/>
@@ -19402,34 +19457,49 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="117"/>
-      <c r="B47" s="124" t="s">
+      <c r="B47" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="122">
+      <c r="C47" s="143">
         <f>(C41*10)/1000</f>
         <v>4.285714285714286E-4</v>
       </c>
-      <c r="D47" s="120">
+      <c r="D47" s="143">
         <v>3.7500000000000006E-4</v>
       </c>
-      <c r="E47" s="121">
+      <c r="E47" s="143">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="F47" s="122">
+      <c r="F47" s="143">
         <v>1.25E-3</v>
       </c>
-      <c r="G47" s="122">
+      <c r="G47" s="143">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="H47" s="126"/>
-      <c r="I47" s="127"/>
-      <c r="J47" s="125"/>
-      <c r="K47" s="125"/>
-      <c r="L47" s="125"/>
-      <c r="M47" s="125"/>
-      <c r="N47" s="125"/>
-      <c r="O47" s="125"/>
-      <c r="P47" s="125"/>
+      <c r="H47" s="142">
+        <f>(H41*10)/1000</f>
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="I47" s="142">
+        <f t="shared" ref="I47:L47" si="30">(I41*10)/1000</f>
+        <v>3.5000000000000005E-4</v>
+      </c>
+      <c r="J47" s="142">
+        <f t="shared" si="30"/>
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="K47" s="142">
+        <f t="shared" si="30"/>
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="L47" s="142">
+        <f t="shared" si="30"/>
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="M47" s="123"/>
+      <c r="N47" s="123"/>
+      <c r="O47" s="123"/>
+      <c r="P47" s="123"/>
       <c r="Q47" s="117"/>
       <c r="R47" s="117"/>
       <c r="S47" s="117"/>
@@ -19437,31 +19507,31 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="117"/>
-      <c r="B48" s="124" t="s">
+      <c r="B48" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="122">
+      <c r="C48" s="143">
         <v>0.01</v>
       </c>
-      <c r="D48" s="120">
+      <c r="D48" s="143">
         <v>5.6250000000000007E-3</v>
       </c>
       <c r="E48" s="121"/>
-      <c r="F48" s="122">
+      <c r="F48" s="143">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G48" s="122">
+      <c r="G48" s="143">
         <v>0.01</v>
       </c>
-      <c r="H48" s="126"/>
-      <c r="I48" s="127"/>
-      <c r="J48" s="125"/>
-      <c r="K48" s="125"/>
-      <c r="L48" s="125"/>
-      <c r="M48" s="125"/>
-      <c r="N48" s="125"/>
-      <c r="O48" s="125"/>
-      <c r="P48" s="125"/>
+      <c r="H48" s="124"/>
+      <c r="I48" s="125"/>
+      <c r="J48" s="123"/>
+      <c r="K48" s="123"/>
+      <c r="L48" s="123"/>
+      <c r="M48" s="123"/>
+      <c r="N48" s="123"/>
+      <c r="O48" s="123"/>
+      <c r="P48" s="123"/>
       <c r="Q48" s="117"/>
       <c r="R48" s="117"/>
       <c r="S48" s="117"/>
@@ -19469,31 +19539,31 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="117"/>
-      <c r="B49" s="124" t="s">
+      <c r="B49" s="122" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="122">
+      <c r="C49" s="143">
         <v>1.6E-2</v>
       </c>
-      <c r="D49" s="120">
+      <c r="D49" s="143">
         <v>6.7500000000000008E-3</v>
       </c>
       <c r="E49" s="121"/>
-      <c r="F49" s="122">
+      <c r="F49" s="143">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G49" s="122">
+      <c r="G49" s="143">
         <v>1.6E-2</v>
       </c>
-      <c r="H49" s="126"/>
-      <c r="I49" s="127"/>
-      <c r="J49" s="125"/>
-      <c r="K49" s="125"/>
-      <c r="L49" s="125"/>
-      <c r="M49" s="125"/>
-      <c r="N49" s="125"/>
-      <c r="O49" s="125"/>
-      <c r="P49" s="125"/>
+      <c r="H49" s="124"/>
+      <c r="I49" s="125"/>
+      <c r="J49" s="123"/>
+      <c r="K49" s="123"/>
+      <c r="L49" s="123"/>
+      <c r="M49" s="123"/>
+      <c r="N49" s="123"/>
+      <c r="O49" s="123"/>
+      <c r="P49" s="123"/>
       <c r="Q49" s="117"/>
       <c r="R49" s="117"/>
       <c r="S49" s="117"/>
@@ -19501,32 +19571,32 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="117"/>
-      <c r="B50" s="128" t="s">
+      <c r="B50" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="122">
+      <c r="C50" s="143">
         <f>(C41*30)/1000</f>
         <v>1.2857142857142859E-3</v>
       </c>
-      <c r="D50" s="120">
+      <c r="D50" s="143">
         <v>9.3750000000000007E-4</v>
       </c>
       <c r="E50" s="121"/>
-      <c r="F50" s="122">
+      <c r="F50" s="143">
         <v>1.8749999999999999E-3</v>
       </c>
-      <c r="G50" s="122">
+      <c r="G50" s="143">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="H50" s="126"/>
-      <c r="I50" s="127"/>
-      <c r="J50" s="125"/>
-      <c r="K50" s="125"/>
-      <c r="L50" s="125"/>
-      <c r="M50" s="125"/>
-      <c r="N50" s="125"/>
-      <c r="O50" s="125"/>
-      <c r="P50" s="125"/>
+      <c r="H50" s="124"/>
+      <c r="I50" s="125"/>
+      <c r="J50" s="123"/>
+      <c r="K50" s="123"/>
+      <c r="L50" s="123"/>
+      <c r="M50" s="123"/>
+      <c r="N50" s="123"/>
+      <c r="O50" s="123"/>
+      <c r="P50" s="123"/>
       <c r="Q50" s="117"/>
       <c r="R50" s="117"/>
       <c r="S50" s="117"/>
@@ -19534,27 +19604,27 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="117"/>
-      <c r="B51" s="129" t="s">
+      <c r="B51" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="130"/>
-      <c r="D51" s="120">
+      <c r="C51" s="128"/>
+      <c r="D51" s="143">
         <v>2.0625000000000005E-3</v>
       </c>
       <c r="E51" s="121"/>
-      <c r="F51" s="130">
+      <c r="F51" s="143">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G51" s="126"/>
-      <c r="H51" s="126"/>
-      <c r="I51" s="127"/>
-      <c r="J51" s="125"/>
-      <c r="K51" s="125"/>
-      <c r="L51" s="125"/>
-      <c r="M51" s="125"/>
-      <c r="N51" s="125"/>
-      <c r="O51" s="125"/>
-      <c r="P51" s="125"/>
+      <c r="G51" s="124"/>
+      <c r="H51" s="124"/>
+      <c r="I51" s="125"/>
+      <c r="J51" s="123"/>
+      <c r="K51" s="123"/>
+      <c r="L51" s="123"/>
+      <c r="M51" s="123"/>
+      <c r="N51" s="123"/>
+      <c r="O51" s="123"/>
+      <c r="P51" s="123"/>
       <c r="Q51" s="117"/>
       <c r="R51" s="117"/>
       <c r="S51" s="117"/>
@@ -19562,27 +19632,27 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="117"/>
-      <c r="B52" s="128" t="s">
+      <c r="B52" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="130"/>
-      <c r="D52" s="131">
+      <c r="C52" s="128"/>
+      <c r="D52" s="143">
         <v>1.6875000000000002E-3</v>
       </c>
-      <c r="E52" s="132"/>
-      <c r="F52" s="130">
+      <c r="E52" s="129"/>
+      <c r="F52" s="143">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="G52" s="126"/>
-      <c r="H52" s="126"/>
-      <c r="I52" s="127"/>
-      <c r="J52" s="125"/>
-      <c r="K52" s="125"/>
-      <c r="L52" s="125"/>
-      <c r="M52" s="125"/>
-      <c r="N52" s="125"/>
-      <c r="O52" s="125"/>
-      <c r="P52" s="125"/>
+      <c r="G52" s="124"/>
+      <c r="H52" s="124"/>
+      <c r="I52" s="125"/>
+      <c r="J52" s="123"/>
+      <c r="K52" s="123"/>
+      <c r="L52" s="123"/>
+      <c r="M52" s="123"/>
+      <c r="N52" s="123"/>
+      <c r="O52" s="123"/>
+      <c r="P52" s="123"/>
       <c r="Q52" s="117"/>
       <c r="R52" s="117"/>
       <c r="S52" s="117"/>
@@ -19590,27 +19660,27 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="117"/>
-      <c r="B53" s="128" t="s">
+      <c r="B53" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="130"/>
-      <c r="D53" s="120">
+      <c r="C53" s="128"/>
+      <c r="D53" s="143">
         <v>1.0500000000000002E-2</v>
       </c>
       <c r="E53" s="120"/>
-      <c r="F53" s="130">
+      <c r="F53" s="143">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G53" s="126"/>
-      <c r="H53" s="126"/>
-      <c r="I53" s="127"/>
-      <c r="J53" s="125"/>
-      <c r="K53" s="125"/>
-      <c r="L53" s="125"/>
-      <c r="M53" s="125"/>
-      <c r="N53" s="125"/>
-      <c r="O53" s="125"/>
-      <c r="P53" s="125"/>
+      <c r="G53" s="124"/>
+      <c r="H53" s="124"/>
+      <c r="I53" s="125"/>
+      <c r="J53" s="123"/>
+      <c r="K53" s="123"/>
+      <c r="L53" s="123"/>
+      <c r="M53" s="123"/>
+      <c r="N53" s="123"/>
+      <c r="O53" s="123"/>
+      <c r="P53" s="123"/>
       <c r="Q53" s="117"/>
       <c r="R53" s="117"/>
       <c r="S53" s="117"/>
@@ -19618,27 +19688,27 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="117"/>
-      <c r="B54" s="129" t="s">
+      <c r="B54" s="127" t="s">
         <v>34</v>
       </c>
       <c r="C54" s="120"/>
-      <c r="D54" s="120">
+      <c r="D54" s="143">
         <v>1.6875000000000002E-3</v>
       </c>
       <c r="E54" s="120"/>
-      <c r="F54" s="120">
+      <c r="F54" s="143">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="G54" s="126"/>
-      <c r="H54" s="126"/>
-      <c r="I54" s="127"/>
-      <c r="J54" s="125"/>
-      <c r="K54" s="125"/>
-      <c r="L54" s="125"/>
-      <c r="M54" s="125"/>
-      <c r="N54" s="125"/>
-      <c r="O54" s="125"/>
-      <c r="P54" s="125"/>
+      <c r="G54" s="124"/>
+      <c r="H54" s="124"/>
+      <c r="I54" s="125"/>
+      <c r="J54" s="123"/>
+      <c r="K54" s="123"/>
+      <c r="L54" s="123"/>
+      <c r="M54" s="123"/>
+      <c r="N54" s="123"/>
+      <c r="O54" s="123"/>
+      <c r="P54" s="123"/>
       <c r="Q54" s="117"/>
       <c r="R54" s="117"/>
       <c r="S54" s="117"/>
@@ -19646,27 +19716,27 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="117"/>
-      <c r="B55" s="129" t="s">
+      <c r="B55" s="127" t="s">
         <v>36</v>
       </c>
       <c r="C55" s="120"/>
-      <c r="D55" s="120">
+      <c r="D55" s="143">
         <v>2.8125000000000003E-3</v>
       </c>
       <c r="E55" s="120"/>
-      <c r="F55" s="120">
+      <c r="F55" s="143">
         <v>6.2500000000000003E-3</v>
       </c>
-      <c r="G55" s="126"/>
-      <c r="H55" s="126"/>
-      <c r="I55" s="127"/>
-      <c r="J55" s="125"/>
-      <c r="K55" s="125"/>
-      <c r="L55" s="125"/>
-      <c r="M55" s="125"/>
-      <c r="N55" s="125"/>
-      <c r="O55" s="125"/>
-      <c r="P55" s="125"/>
+      <c r="G55" s="124"/>
+      <c r="H55" s="124"/>
+      <c r="I55" s="125"/>
+      <c r="J55" s="123"/>
+      <c r="K55" s="123"/>
+      <c r="L55" s="123"/>
+      <c r="M55" s="123"/>
+      <c r="N55" s="123"/>
+      <c r="O55" s="123"/>
+      <c r="P55" s="123"/>
       <c r="Q55" s="117"/>
       <c r="R55" s="117"/>
       <c r="S55" s="117"/>
@@ -19674,27 +19744,27 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="117"/>
-      <c r="B56" s="129" t="s">
+      <c r="B56" s="127" t="s">
         <v>37</v>
       </c>
       <c r="C56" s="120"/>
-      <c r="D56" s="120">
+      <c r="D56" s="143">
         <v>1.5000000000000002E-3</v>
       </c>
       <c r="E56" s="120"/>
-      <c r="F56" s="120">
+      <c r="F56" s="143">
         <v>3.1250000000000002E-3</v>
       </c>
-      <c r="G56" s="126"/>
-      <c r="H56" s="126"/>
-      <c r="I56" s="127"/>
-      <c r="J56" s="125"/>
-      <c r="K56" s="125"/>
-      <c r="L56" s="125"/>
-      <c r="M56" s="125"/>
-      <c r="N56" s="125"/>
-      <c r="O56" s="125"/>
-      <c r="P56" s="125"/>
+      <c r="G56" s="124"/>
+      <c r="H56" s="124"/>
+      <c r="I56" s="125"/>
+      <c r="J56" s="123"/>
+      <c r="K56" s="123"/>
+      <c r="L56" s="123"/>
+      <c r="M56" s="123"/>
+      <c r="N56" s="123"/>
+      <c r="O56" s="123"/>
+      <c r="P56" s="123"/>
       <c r="Q56" s="117"/>
       <c r="R56" s="117"/>
       <c r="S56" s="117"/>
@@ -19702,467 +19772,467 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="117"/>
-      <c r="B57" s="128" t="s">
+      <c r="B57" s="126" t="s">
         <v>146</v>
       </c>
       <c r="C57" s="120"/>
-      <c r="D57" s="120">
+      <c r="D57" s="143">
         <v>2.2500000000000003E-2</v>
       </c>
       <c r="E57" s="120"/>
-      <c r="F57" s="120">
+      <c r="F57" s="143">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G57" s="126"/>
-      <c r="H57" s="126"/>
-      <c r="I57" s="126"/>
-      <c r="J57" s="126"/>
-      <c r="K57" s="126"/>
-      <c r="L57" s="126"/>
-      <c r="M57" s="127"/>
-      <c r="N57" s="125"/>
-      <c r="O57" s="125"/>
-      <c r="P57" s="125"/>
-      <c r="Q57" s="125"/>
-      <c r="R57" s="125"/>
-      <c r="S57" s="125"/>
-      <c r="T57" s="125"/>
+      <c r="G57" s="124"/>
+      <c r="H57" s="124"/>
+      <c r="I57" s="124"/>
+      <c r="J57" s="124"/>
+      <c r="K57" s="124"/>
+      <c r="L57" s="124"/>
+      <c r="M57" s="125"/>
+      <c r="N57" s="123"/>
+      <c r="O57" s="123"/>
+      <c r="P57" s="123"/>
+      <c r="Q57" s="123"/>
+      <c r="R57" s="123"/>
+      <c r="S57" s="123"/>
+      <c r="T57" s="123"/>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="117"/>
-      <c r="B58" s="133" t="s">
+      <c r="B58" s="130" t="s">
         <v>240</v>
       </c>
-      <c r="C58" s="126"/>
-      <c r="D58" s="126"/>
-      <c r="E58" s="126"/>
-      <c r="F58" s="126"/>
-      <c r="G58" s="126"/>
-      <c r="H58" s="126"/>
-      <c r="I58" s="126">
+      <c r="C58" s="124"/>
+      <c r="D58" s="124"/>
+      <c r="E58" s="124"/>
+      <c r="F58" s="124"/>
+      <c r="G58" s="124"/>
+      <c r="H58" s="124"/>
+      <c r="I58" s="142">
         <v>1.2E-2</v>
       </c>
-      <c r="J58" s="126"/>
-      <c r="K58" s="126"/>
-      <c r="L58" s="126"/>
-      <c r="M58" s="127"/>
-      <c r="N58" s="125"/>
-      <c r="O58" s="125"/>
-      <c r="P58" s="125"/>
-      <c r="Q58" s="125"/>
-      <c r="R58" s="125"/>
-      <c r="S58" s="125"/>
-      <c r="T58" s="125"/>
+      <c r="J58" s="124"/>
+      <c r="K58" s="124"/>
+      <c r="L58" s="124"/>
+      <c r="M58" s="125"/>
+      <c r="N58" s="123"/>
+      <c r="O58" s="123"/>
+      <c r="P58" s="123"/>
+      <c r="Q58" s="123"/>
+      <c r="R58" s="123"/>
+      <c r="S58" s="123"/>
+      <c r="T58" s="123"/>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="117"/>
-      <c r="B59" s="133" t="s">
+      <c r="B59" s="130" t="s">
         <v>241</v>
       </c>
-      <c r="C59" s="126"/>
-      <c r="D59" s="126"/>
-      <c r="E59" s="126"/>
-      <c r="F59" s="126"/>
-      <c r="G59" s="126"/>
-      <c r="H59" s="126"/>
-      <c r="I59" s="126"/>
-      <c r="J59" s="126">
+      <c r="C59" s="124"/>
+      <c r="D59" s="124"/>
+      <c r="E59" s="124"/>
+      <c r="F59" s="124"/>
+      <c r="G59" s="124"/>
+      <c r="H59" s="124"/>
+      <c r="I59" s="124"/>
+      <c r="J59" s="142">
         <v>1.2E-2</v>
       </c>
-      <c r="K59" s="126"/>
-      <c r="L59" s="126"/>
-      <c r="M59" s="127"/>
-      <c r="N59" s="125"/>
-      <c r="O59" s="125"/>
-      <c r="P59" s="125"/>
-      <c r="Q59" s="125"/>
-      <c r="R59" s="125"/>
-      <c r="S59" s="125"/>
-      <c r="T59" s="125"/>
+      <c r="K59" s="124"/>
+      <c r="L59" s="124"/>
+      <c r="M59" s="125"/>
+      <c r="N59" s="123"/>
+      <c r="O59" s="123"/>
+      <c r="P59" s="123"/>
+      <c r="Q59" s="123"/>
+      <c r="R59" s="123"/>
+      <c r="S59" s="123"/>
+      <c r="T59" s="123"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="117"/>
-      <c r="B60" s="124" t="s">
+      <c r="B60" s="122" t="s">
         <v>264</v>
       </c>
-      <c r="C60" s="126"/>
-      <c r="D60" s="126"/>
-      <c r="E60" s="126"/>
-      <c r="F60" s="126"/>
-      <c r="G60" s="126"/>
-      <c r="H60" s="126"/>
-      <c r="I60" s="126"/>
-      <c r="J60" s="126"/>
-      <c r="K60" s="126"/>
-      <c r="L60" s="126"/>
-      <c r="M60" s="127"/>
-      <c r="N60" s="125"/>
-      <c r="O60" s="125"/>
-      <c r="P60" s="125"/>
-      <c r="Q60" s="125"/>
-      <c r="R60" s="125"/>
-      <c r="S60" s="125"/>
-      <c r="T60" s="125"/>
+      <c r="C60" s="124"/>
+      <c r="D60" s="124"/>
+      <c r="E60" s="124"/>
+      <c r="F60" s="124"/>
+      <c r="G60" s="124"/>
+      <c r="H60" s="124"/>
+      <c r="I60" s="124"/>
+      <c r="J60" s="124"/>
+      <c r="K60" s="124"/>
+      <c r="L60" s="124"/>
+      <c r="M60" s="125"/>
+      <c r="N60" s="123"/>
+      <c r="O60" s="123"/>
+      <c r="P60" s="123"/>
+      <c r="Q60" s="123"/>
+      <c r="R60" s="123"/>
+      <c r="S60" s="123"/>
+      <c r="T60" s="123"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="117"/>
-      <c r="B61" s="124" t="s">
+      <c r="B61" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="126"/>
-      <c r="D61" s="126"/>
-      <c r="E61" s="126"/>
-      <c r="F61" s="126"/>
-      <c r="G61" s="126"/>
-      <c r="H61" s="126"/>
-      <c r="I61" s="126"/>
-      <c r="J61" s="126"/>
-      <c r="K61" s="126"/>
-      <c r="L61" s="126"/>
-      <c r="M61" s="127"/>
-      <c r="N61" s="125"/>
-      <c r="O61" s="125"/>
-      <c r="P61" s="125"/>
-      <c r="Q61" s="125"/>
-      <c r="R61" s="125"/>
-      <c r="S61" s="125"/>
-      <c r="T61" s="125"/>
+      <c r="C61" s="124"/>
+      <c r="D61" s="124"/>
+      <c r="E61" s="124"/>
+      <c r="F61" s="124"/>
+      <c r="G61" s="124"/>
+      <c r="H61" s="124"/>
+      <c r="I61" s="124"/>
+      <c r="J61" s="124"/>
+      <c r="K61" s="124"/>
+      <c r="L61" s="124"/>
+      <c r="M61" s="125"/>
+      <c r="N61" s="123"/>
+      <c r="O61" s="123"/>
+      <c r="P61" s="123"/>
+      <c r="Q61" s="123"/>
+      <c r="R61" s="123"/>
+      <c r="S61" s="123"/>
+      <c r="T61" s="123"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="117"/>
-      <c r="B62" s="124" t="s">
+      <c r="B62" s="122" t="s">
         <v>188</v>
       </c>
-      <c r="C62" s="126"/>
-      <c r="D62" s="126"/>
-      <c r="E62" s="126"/>
-      <c r="F62" s="126"/>
-      <c r="G62" s="126"/>
-      <c r="H62" s="126"/>
-      <c r="I62" s="126"/>
-      <c r="J62" s="126"/>
-      <c r="K62" s="126"/>
-      <c r="L62" s="126"/>
-      <c r="M62" s="127"/>
-      <c r="N62" s="125"/>
-      <c r="O62" s="125"/>
-      <c r="P62" s="125"/>
-      <c r="Q62" s="125"/>
-      <c r="R62" s="125"/>
-      <c r="S62" s="125"/>
-      <c r="T62" s="125"/>
+      <c r="C62" s="124"/>
+      <c r="D62" s="124"/>
+      <c r="E62" s="124"/>
+      <c r="F62" s="124"/>
+      <c r="G62" s="124"/>
+      <c r="H62" s="124"/>
+      <c r="I62" s="124"/>
+      <c r="J62" s="124"/>
+      <c r="K62" s="124"/>
+      <c r="L62" s="124"/>
+      <c r="M62" s="125"/>
+      <c r="N62" s="123"/>
+      <c r="O62" s="123"/>
+      <c r="P62" s="123"/>
+      <c r="Q62" s="123"/>
+      <c r="R62" s="123"/>
+      <c r="S62" s="123"/>
+      <c r="T62" s="123"/>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="117"/>
-      <c r="B63" s="124" t="s">
+      <c r="B63" s="122" t="s">
         <v>265</v>
       </c>
-      <c r="C63" s="126"/>
-      <c r="D63" s="126"/>
-      <c r="E63" s="126"/>
-      <c r="F63" s="126"/>
-      <c r="G63" s="126"/>
-      <c r="H63" s="126"/>
-      <c r="I63" s="126"/>
-      <c r="J63" s="126"/>
-      <c r="K63" s="126"/>
-      <c r="L63" s="126"/>
-      <c r="M63" s="127"/>
-      <c r="N63" s="125"/>
-      <c r="O63" s="125"/>
-      <c r="P63" s="125"/>
-      <c r="Q63" s="125"/>
-      <c r="R63" s="125"/>
-      <c r="S63" s="125"/>
-      <c r="T63" s="125"/>
+      <c r="C63" s="124"/>
+      <c r="D63" s="124"/>
+      <c r="E63" s="124"/>
+      <c r="F63" s="124"/>
+      <c r="G63" s="124"/>
+      <c r="H63" s="124"/>
+      <c r="I63" s="124"/>
+      <c r="J63" s="124"/>
+      <c r="K63" s="124"/>
+      <c r="L63" s="124"/>
+      <c r="M63" s="125"/>
+      <c r="N63" s="123"/>
+      <c r="O63" s="123"/>
+      <c r="P63" s="123"/>
+      <c r="Q63" s="123"/>
+      <c r="R63" s="123"/>
+      <c r="S63" s="123"/>
+      <c r="T63" s="123"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="117"/>
-      <c r="B64" s="124" t="s">
+      <c r="B64" s="122" t="s">
         <v>266</v>
       </c>
-      <c r="C64" s="126"/>
-      <c r="D64" s="126"/>
-      <c r="E64" s="126"/>
-      <c r="F64" s="126"/>
-      <c r="G64" s="126"/>
-      <c r="H64" s="126"/>
-      <c r="I64" s="126"/>
-      <c r="J64" s="126"/>
-      <c r="K64" s="126"/>
-      <c r="L64" s="126"/>
-      <c r="M64" s="127"/>
-      <c r="N64" s="125"/>
-      <c r="O64" s="125"/>
-      <c r="P64" s="125"/>
-      <c r="Q64" s="125"/>
-      <c r="R64" s="125"/>
-      <c r="S64" s="125"/>
-      <c r="T64" s="125"/>
+      <c r="C64" s="124"/>
+      <c r="D64" s="124"/>
+      <c r="E64" s="124"/>
+      <c r="F64" s="124"/>
+      <c r="G64" s="124"/>
+      <c r="H64" s="124"/>
+      <c r="I64" s="124"/>
+      <c r="J64" s="124"/>
+      <c r="K64" s="124"/>
+      <c r="L64" s="124"/>
+      <c r="M64" s="125"/>
+      <c r="N64" s="123"/>
+      <c r="O64" s="123"/>
+      <c r="P64" s="123"/>
+      <c r="Q64" s="123"/>
+      <c r="R64" s="123"/>
+      <c r="S64" s="123"/>
+      <c r="T64" s="123"/>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="117"/>
-      <c r="B65" s="124" t="s">
+      <c r="B65" s="122" t="s">
         <v>172</v>
       </c>
-      <c r="C65" s="126"/>
-      <c r="D65" s="126"/>
-      <c r="E65" s="126"/>
-      <c r="F65" s="126"/>
-      <c r="G65" s="126"/>
-      <c r="H65" s="126"/>
-      <c r="I65" s="126"/>
-      <c r="J65" s="126"/>
-      <c r="K65" s="126"/>
-      <c r="L65" s="126"/>
-      <c r="M65" s="127"/>
-      <c r="N65" s="125"/>
-      <c r="O65" s="125"/>
-      <c r="P65" s="125"/>
-      <c r="Q65" s="125"/>
-      <c r="R65" s="125"/>
-      <c r="S65" s="125"/>
-      <c r="T65" s="125"/>
+      <c r="C65" s="124"/>
+      <c r="D65" s="124"/>
+      <c r="E65" s="124"/>
+      <c r="F65" s="124"/>
+      <c r="G65" s="124"/>
+      <c r="H65" s="124"/>
+      <c r="I65" s="124"/>
+      <c r="J65" s="124"/>
+      <c r="K65" s="124"/>
+      <c r="L65" s="124"/>
+      <c r="M65" s="125"/>
+      <c r="N65" s="123"/>
+      <c r="O65" s="123"/>
+      <c r="P65" s="123"/>
+      <c r="Q65" s="123"/>
+      <c r="R65" s="123"/>
+      <c r="S65" s="123"/>
+      <c r="T65" s="123"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="117"/>
-      <c r="B66" s="124" t="s">
+      <c r="B66" s="122" t="s">
         <v>267</v>
       </c>
-      <c r="C66" s="126"/>
-      <c r="D66" s="126"/>
-      <c r="E66" s="126"/>
-      <c r="F66" s="126"/>
-      <c r="G66" s="126"/>
-      <c r="H66" s="126"/>
-      <c r="I66" s="126"/>
-      <c r="J66" s="126"/>
-      <c r="K66" s="126"/>
-      <c r="L66" s="126"/>
-      <c r="M66" s="127"/>
-      <c r="N66" s="125"/>
-      <c r="O66" s="125"/>
-      <c r="P66" s="125"/>
-      <c r="Q66" s="125"/>
-      <c r="R66" s="125"/>
-      <c r="S66" s="125"/>
-      <c r="T66" s="125"/>
+      <c r="C66" s="124"/>
+      <c r="D66" s="124"/>
+      <c r="E66" s="124"/>
+      <c r="F66" s="124"/>
+      <c r="G66" s="124"/>
+      <c r="H66" s="124"/>
+      <c r="I66" s="124"/>
+      <c r="J66" s="124"/>
+      <c r="K66" s="124"/>
+      <c r="L66" s="124"/>
+      <c r="M66" s="125"/>
+      <c r="N66" s="123"/>
+      <c r="O66" s="123"/>
+      <c r="P66" s="123"/>
+      <c r="Q66" s="123"/>
+      <c r="R66" s="123"/>
+      <c r="S66" s="123"/>
+      <c r="T66" s="123"/>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="117"/>
-      <c r="B67" s="124" t="s">
+      <c r="B67" s="122" t="s">
         <v>72</v>
       </c>
-      <c r="C67" s="126"/>
-      <c r="D67" s="126"/>
-      <c r="E67" s="126"/>
-      <c r="F67" s="126"/>
-      <c r="G67" s="126"/>
-      <c r="H67" s="126"/>
-      <c r="I67" s="126"/>
-      <c r="J67" s="126"/>
-      <c r="K67" s="126"/>
-      <c r="L67" s="126"/>
-      <c r="M67" s="127"/>
-      <c r="N67" s="125"/>
-      <c r="O67" s="125"/>
-      <c r="P67" s="125"/>
-      <c r="Q67" s="125"/>
-      <c r="R67" s="125"/>
-      <c r="S67" s="125"/>
-      <c r="T67" s="125"/>
+      <c r="C67" s="124"/>
+      <c r="D67" s="124"/>
+      <c r="E67" s="124"/>
+      <c r="F67" s="124"/>
+      <c r="G67" s="124"/>
+      <c r="H67" s="124"/>
+      <c r="I67" s="124"/>
+      <c r="J67" s="124"/>
+      <c r="K67" s="124"/>
+      <c r="L67" s="124"/>
+      <c r="M67" s="125"/>
+      <c r="N67" s="123"/>
+      <c r="O67" s="123"/>
+      <c r="P67" s="123"/>
+      <c r="Q67" s="123"/>
+      <c r="R67" s="123"/>
+      <c r="S67" s="123"/>
+      <c r="T67" s="123"/>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="117"/>
-      <c r="B68" s="124" t="s">
+      <c r="B68" s="122" t="s">
         <v>268</v>
       </c>
-      <c r="C68" s="126"/>
-      <c r="D68" s="126"/>
-      <c r="E68" s="126"/>
-      <c r="F68" s="126"/>
-      <c r="G68" s="126"/>
-      <c r="H68" s="126"/>
-      <c r="I68" s="126"/>
-      <c r="J68" s="126"/>
-      <c r="K68" s="126"/>
-      <c r="L68" s="126"/>
-      <c r="M68" s="127"/>
-      <c r="N68" s="125"/>
-      <c r="O68" s="125"/>
-      <c r="P68" s="125"/>
-      <c r="Q68" s="125"/>
-      <c r="R68" s="125"/>
-      <c r="S68" s="125"/>
-      <c r="T68" s="125"/>
+      <c r="C68" s="124"/>
+      <c r="D68" s="124"/>
+      <c r="E68" s="124"/>
+      <c r="F68" s="124"/>
+      <c r="G68" s="124"/>
+      <c r="H68" s="124"/>
+      <c r="I68" s="124"/>
+      <c r="J68" s="124"/>
+      <c r="K68" s="124"/>
+      <c r="L68" s="124"/>
+      <c r="M68" s="125"/>
+      <c r="N68" s="123"/>
+      <c r="O68" s="123"/>
+      <c r="P68" s="123"/>
+      <c r="Q68" s="123"/>
+      <c r="R68" s="123"/>
+      <c r="S68" s="123"/>
+      <c r="T68" s="123"/>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="117"/>
-      <c r="B69" s="124" t="s">
+      <c r="B69" s="122" t="s">
         <v>269</v>
       </c>
-      <c r="C69" s="126"/>
-      <c r="D69" s="126"/>
-      <c r="E69" s="126"/>
-      <c r="F69" s="126"/>
-      <c r="G69" s="126"/>
-      <c r="H69" s="126"/>
-      <c r="I69" s="126"/>
-      <c r="J69" s="126"/>
-      <c r="K69" s="126"/>
-      <c r="L69" s="126"/>
-      <c r="M69" s="127"/>
-      <c r="N69" s="125"/>
-      <c r="O69" s="125"/>
-      <c r="P69" s="125"/>
-      <c r="Q69" s="125"/>
-      <c r="R69" s="125"/>
-      <c r="S69" s="125"/>
-      <c r="T69" s="125"/>
+      <c r="C69" s="124"/>
+      <c r="D69" s="124"/>
+      <c r="E69" s="124"/>
+      <c r="F69" s="124"/>
+      <c r="G69" s="124"/>
+      <c r="H69" s="124"/>
+      <c r="I69" s="124"/>
+      <c r="J69" s="124"/>
+      <c r="K69" s="124"/>
+      <c r="L69" s="124"/>
+      <c r="M69" s="125"/>
+      <c r="N69" s="123"/>
+      <c r="O69" s="123"/>
+      <c r="P69" s="123"/>
+      <c r="Q69" s="123"/>
+      <c r="R69" s="123"/>
+      <c r="S69" s="123"/>
+      <c r="T69" s="123"/>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="117"/>
-      <c r="B70" s="124" t="s">
+      <c r="B70" s="122" t="s">
         <v>105</v>
       </c>
-      <c r="C70" s="126"/>
-      <c r="D70" s="126"/>
-      <c r="E70" s="126"/>
-      <c r="F70" s="126"/>
-      <c r="G70" s="126"/>
-      <c r="H70" s="126"/>
-      <c r="I70" s="126"/>
-      <c r="J70" s="126"/>
-      <c r="K70" s="126"/>
-      <c r="L70" s="126"/>
-      <c r="M70" s="127"/>
-      <c r="N70" s="125"/>
-      <c r="O70" s="125"/>
-      <c r="P70" s="125"/>
-      <c r="Q70" s="125"/>
-      <c r="R70" s="125"/>
-      <c r="S70" s="125"/>
-      <c r="T70" s="125"/>
+      <c r="C70" s="124"/>
+      <c r="D70" s="124"/>
+      <c r="E70" s="124"/>
+      <c r="F70" s="124"/>
+      <c r="G70" s="124"/>
+      <c r="H70" s="124"/>
+      <c r="I70" s="124"/>
+      <c r="J70" s="124"/>
+      <c r="K70" s="124"/>
+      <c r="L70" s="124"/>
+      <c r="M70" s="125"/>
+      <c r="N70" s="123"/>
+      <c r="O70" s="123"/>
+      <c r="P70" s="123"/>
+      <c r="Q70" s="123"/>
+      <c r="R70" s="123"/>
+      <c r="S70" s="123"/>
+      <c r="T70" s="123"/>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="117"/>
-      <c r="B71" s="124" t="s">
+      <c r="B71" s="122" t="s">
         <v>270</v>
       </c>
-      <c r="C71" s="126"/>
-      <c r="D71" s="126"/>
-      <c r="E71" s="126"/>
-      <c r="F71" s="126"/>
-      <c r="G71" s="126"/>
-      <c r="H71" s="126"/>
-      <c r="I71" s="126"/>
-      <c r="J71" s="126"/>
-      <c r="K71" s="126"/>
-      <c r="L71" s="126"/>
-      <c r="M71" s="127"/>
-      <c r="N71" s="125"/>
-      <c r="O71" s="125"/>
-      <c r="P71" s="125"/>
-      <c r="Q71" s="125"/>
-      <c r="R71" s="125"/>
-      <c r="S71" s="125"/>
-      <c r="T71" s="125"/>
+      <c r="C71" s="124"/>
+      <c r="D71" s="124"/>
+      <c r="E71" s="124"/>
+      <c r="F71" s="124"/>
+      <c r="G71" s="124"/>
+      <c r="H71" s="124"/>
+      <c r="I71" s="124"/>
+      <c r="J71" s="124"/>
+      <c r="K71" s="124"/>
+      <c r="L71" s="124"/>
+      <c r="M71" s="125"/>
+      <c r="N71" s="123"/>
+      <c r="O71" s="123"/>
+      <c r="P71" s="123"/>
+      <c r="Q71" s="123"/>
+      <c r="R71" s="123"/>
+      <c r="S71" s="123"/>
+      <c r="T71" s="123"/>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="117"/>
-      <c r="B72" s="124" t="s">
+      <c r="B72" s="122" t="s">
         <v>271</v>
       </c>
-      <c r="C72" s="126"/>
-      <c r="D72" s="126"/>
-      <c r="E72" s="126"/>
-      <c r="F72" s="126"/>
-      <c r="G72" s="126"/>
-      <c r="H72" s="126"/>
-      <c r="I72" s="126"/>
-      <c r="J72" s="126"/>
-      <c r="K72" s="126"/>
-      <c r="L72" s="126"/>
-      <c r="M72" s="127"/>
-      <c r="N72" s="125"/>
-      <c r="O72" s="125"/>
-      <c r="P72" s="125"/>
-      <c r="Q72" s="125"/>
-      <c r="R72" s="125"/>
-      <c r="S72" s="125"/>
-      <c r="T72" s="125"/>
+      <c r="C72" s="124"/>
+      <c r="D72" s="124"/>
+      <c r="E72" s="124"/>
+      <c r="F72" s="124"/>
+      <c r="G72" s="124"/>
+      <c r="H72" s="124"/>
+      <c r="I72" s="124"/>
+      <c r="J72" s="124"/>
+      <c r="K72" s="124"/>
+      <c r="L72" s="124"/>
+      <c r="M72" s="125"/>
+      <c r="N72" s="123"/>
+      <c r="O72" s="123"/>
+      <c r="P72" s="123"/>
+      <c r="Q72" s="123"/>
+      <c r="R72" s="123"/>
+      <c r="S72" s="123"/>
+      <c r="T72" s="123"/>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="117"/>
-      <c r="B73" s="124" t="s">
+      <c r="B73" s="122" t="s">
         <v>150</v>
       </c>
-      <c r="C73" s="126"/>
-      <c r="D73" s="126"/>
-      <c r="E73" s="126"/>
-      <c r="F73" s="126"/>
-      <c r="G73" s="126"/>
-      <c r="H73" s="126"/>
-      <c r="I73" s="126"/>
-      <c r="J73" s="126"/>
-      <c r="K73" s="126"/>
-      <c r="L73" s="126"/>
-      <c r="M73" s="127"/>
-      <c r="N73" s="125"/>
-      <c r="O73" s="125"/>
-      <c r="P73" s="125"/>
-      <c r="Q73" s="125"/>
-      <c r="R73" s="125"/>
-      <c r="S73" s="125"/>
-      <c r="T73" s="125"/>
+      <c r="C73" s="124"/>
+      <c r="D73" s="124"/>
+      <c r="E73" s="124"/>
+      <c r="F73" s="124"/>
+      <c r="G73" s="124"/>
+      <c r="H73" s="124"/>
+      <c r="I73" s="124"/>
+      <c r="J73" s="124"/>
+      <c r="K73" s="124"/>
+      <c r="L73" s="124"/>
+      <c r="M73" s="125"/>
+      <c r="N73" s="123"/>
+      <c r="O73" s="123"/>
+      <c r="P73" s="123"/>
+      <c r="Q73" s="123"/>
+      <c r="R73" s="123"/>
+      <c r="S73" s="123"/>
+      <c r="T73" s="123"/>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="117"/>
-      <c r="B74" s="124" t="s">
+      <c r="B74" s="122" t="s">
         <v>152</v>
       </c>
-      <c r="C74" s="126"/>
-      <c r="D74" s="126"/>
-      <c r="E74" s="126"/>
-      <c r="F74" s="126"/>
-      <c r="G74" s="126"/>
-      <c r="H74" s="126"/>
-      <c r="I74" s="126"/>
-      <c r="J74" s="126"/>
-      <c r="K74" s="126"/>
-      <c r="L74" s="126"/>
-      <c r="M74" s="127"/>
-      <c r="N74" s="125"/>
-      <c r="O74" s="125"/>
-      <c r="P74" s="125"/>
-      <c r="Q74" s="125"/>
-      <c r="R74" s="125"/>
-      <c r="S74" s="125"/>
-      <c r="T74" s="125"/>
+      <c r="C74" s="124"/>
+      <c r="D74" s="124"/>
+      <c r="E74" s="124"/>
+      <c r="F74" s="124"/>
+      <c r="G74" s="124"/>
+      <c r="H74" s="124"/>
+      <c r="I74" s="124"/>
+      <c r="J74" s="124"/>
+      <c r="K74" s="124"/>
+      <c r="L74" s="124"/>
+      <c r="M74" s="125"/>
+      <c r="N74" s="123"/>
+      <c r="O74" s="123"/>
+      <c r="P74" s="123"/>
+      <c r="Q74" s="123"/>
+      <c r="R74" s="123"/>
+      <c r="S74" s="123"/>
+      <c r="T74" s="123"/>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="117"/>
-      <c r="B75" s="124" t="s">
+      <c r="B75" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="C75" s="126"/>
-      <c r="D75" s="126"/>
-      <c r="E75" s="126"/>
-      <c r="F75" s="126"/>
-      <c r="G75" s="126"/>
-      <c r="H75" s="126"/>
-      <c r="I75" s="126"/>
-      <c r="J75" s="126"/>
-      <c r="K75" s="126"/>
-      <c r="L75" s="126"/>
-      <c r="M75" s="127"/>
-      <c r="N75" s="125"/>
-      <c r="O75" s="125"/>
-      <c r="P75" s="125"/>
-      <c r="Q75" s="125"/>
-      <c r="R75" s="125"/>
-      <c r="S75" s="125"/>
-      <c r="T75" s="125"/>
+      <c r="C75" s="124"/>
+      <c r="D75" s="124"/>
+      <c r="E75" s="124"/>
+      <c r="F75" s="124"/>
+      <c r="G75" s="124"/>
+      <c r="H75" s="124"/>
+      <c r="I75" s="124"/>
+      <c r="J75" s="124"/>
+      <c r="K75" s="124"/>
+      <c r="L75" s="124"/>
+      <c r="M75" s="125"/>
+      <c r="N75" s="123"/>
+      <c r="O75" s="123"/>
+      <c r="P75" s="123"/>
+      <c r="Q75" s="123"/>
+      <c r="R75" s="123"/>
+      <c r="S75" s="123"/>
+      <c r="T75" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -21093,10 +21163,10 @@
       <c r="P2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="137" t="s">
+      <c r="R2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="S2" s="137"/>
+      <c r="S2" s="134"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -21158,8 +21228,8 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="P3" s="8"/>
-      <c r="R3" s="137"/>
-      <c r="S3" s="137"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="134"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -21731,10 +21801,10 @@
       <c r="O2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="137" t="s">
+      <c r="Q2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="R2" s="137"/>
+      <c r="R2" s="134"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -21791,8 +21861,8 @@
         <v>1.503E-2</v>
       </c>
       <c r="O3" s="8"/>
-      <c r="Q3" s="137"/>
-      <c r="R3" s="137"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -22018,10 +22088,10 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K1" s="22"/>
-      <c r="M1" s="141" t="s">
+      <c r="M1" s="138" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="141"/>
+      <c r="N1" s="138"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -22067,10 +22137,10 @@
         <v>63</v>
       </c>
       <c r="O2" s="17"/>
-      <c r="P2" s="137" t="s">
+      <c r="P2" s="134" t="s">
         <v>227</v>
       </c>
-      <c r="Q2" s="137"/>
+      <c r="Q2" s="134"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -22129,8 +22199,8 @@
         <v>2.5019999999999997E-2</v>
       </c>
       <c r="O3" s="17"/>
-      <c r="P3" s="137"/>
-      <c r="Q3" s="137"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>

</xml_diff>

<commit_message>
Code for first release
</commit_message>
<xml_diff>
--- a/Documents/Thannickal_Bakers_Working.xlsx
+++ b/Documents/Thannickal_Bakers_Working.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Globocon\BMS\Application\BakeryManagementSystem\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8B0451-86A6-4BA9-9AF8-906C0F01DDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9770755-6836-4417-BB0E-D34CE9E6A122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" firstSheet="1" activeTab="4" xr2:uid="{9EA4B1FA-7DD5-4CCE-97E0-9A7AE5A0A6E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" firstSheet="30" activeTab="35" xr2:uid="{9EA4B1FA-7DD5-4CCE-97E0-9A7AE5A0A6E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="31" r:id="rId1"/>
@@ -48,9 +48,10 @@
     <sheet name="RawMaterials" sheetId="40" r:id="rId33"/>
     <sheet name="Products" sheetId="41" r:id="rId34"/>
     <sheet name="Products_Rawmaterial" sheetId="43" r:id="rId35"/>
+    <sheet name="Report1" sheetId="44" r:id="rId36"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId36"/>
+    <externalReference r:id="rId37"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="329">
   <si>
     <t>Item</t>
   </si>
@@ -1025,6 +1026,30 @@
   </si>
   <si>
     <t>RM MapID</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Team Wise Items Prepration List</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>[OrderDate]</t>
+  </si>
+  <si>
+    <t>Ingrident Name</t>
+  </si>
+  <si>
+    <t>Ingrident Req Qty</t>
+  </si>
+  <si>
+    <t>[TeamName]</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1061,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1141,6 +1166,24 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -1234,7 +1277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1588,12 +1631,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1935,6 +2002,19 @@
     <xf numFmtId="167" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -15959,6 +16039,98 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F45509-B26B-44D6-A57B-9AB7E42E87E5}">
+  <dimension ref="B1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="146" t="s">
+        <v>322</v>
+      </c>
+      <c r="C2" s="147"/>
+      <c r="D2" s="148"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" s="145" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="145" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC33473-5EA2-4215-877C-A76652DD2EEC}">
   <dimension ref="A2:R77"/>
@@ -17374,8 +17546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D55B50-A414-40E8-B274-E34251BCB63C}">
   <dimension ref="A2:Y75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="133" zoomScaleNormal="231" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView topLeftCell="A37" zoomScale="133" zoomScaleNormal="231" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18254,7 +18426,9 @@
       <c r="A26" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="B26" s="21"/>
+      <c r="B26" s="21">
+        <v>1</v>
+      </c>
       <c r="C26" s="9">
         <v>0.5</v>
       </c>
@@ -18330,7 +18504,9 @@
       <c r="A27" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="B27" s="21"/>
+      <c r="B27" s="21">
+        <v>1</v>
+      </c>
       <c r="C27" s="9">
         <v>0.1</v>
       </c>
@@ -20250,8 +20426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75B44F2-5692-3F4F-AB9E-16CFC18BE7AA}">
   <dimension ref="A3:Q23"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21091,7 +21267,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>